<commit_message>
Rename data files so they are informative
</commit_message>
<xml_diff>
--- a/inst/Chaut Example Data_122925_QC.xlsx
+++ b/inst/Chaut Example Data_122925_QC.xlsx
@@ -539,6 +539,16 @@
       <c r="T2" s="2">
         <v>45804</v>
       </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.354); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -599,6 +609,16 @@
       <c r="T3" s="2">
         <v>45804</v>
       </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.434); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -659,6 +679,16 @@
       <c r="T4" s="2">
         <v>45799</v>
       </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.494); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -839,6 +869,16 @@
       <c r="T7" s="2">
         <v>45797</v>
       </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-3.053); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1101,6 +1141,16 @@
       <c r="T11" s="2">
         <v>45799</v>
       </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (2.817); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1433,6 +1483,16 @@
       <c r="T16" s="2">
         <v>45797</v>
       </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.871); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1830,6 +1890,16 @@
       <c r="T22" s="2">
         <v>45799</v>
       </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (8.969); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2080,6 +2150,16 @@
       <c r="T26" s="2">
         <v>45797</v>
       </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-4.07); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2397,6 +2477,16 @@
       <c r="T31" s="2">
         <v>45797</v>
       </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-2.702); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3248,6 +3338,16 @@
       <c r="T44" s="2">
         <v>45812</v>
       </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.364); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3305,6 +3405,16 @@
       <c r="T45" s="2">
         <v>45821</v>
       </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.645); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3476,6 +3586,16 @@
       <c r="T48" s="2">
         <v>45819</v>
       </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (3.21); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4626,6 +4746,16 @@
       <c r="T67" s="2">
         <v>45821</v>
       </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (2.125); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4838,6 +4968,16 @@
       <c r="T71" s="2">
         <v>45819</v>
       </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (8.087); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -5536,6 +5676,16 @@
       <c r="T83" s="2">
         <v>45821</v>
       </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V83" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (6.292); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -5709,6 +5859,16 @@
       <c r="T86" s="2">
         <v>45821</v>
       </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V86" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.185); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -5769,6 +5929,16 @@
       <c r="T87" s="2">
         <v>45817</v>
       </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V87" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.997); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -5829,6 +5999,16 @@
       <c r="T88" s="2">
         <v>45817</v>
       </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V88" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (1.054); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -6787,6 +6967,16 @@
       <c r="T103" s="2">
         <v>45821</v>
       </c>
+      <c r="U103" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V103" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (5.093); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -6857,6 +7047,16 @@
       <c r="T104" s="2">
         <v>45826</v>
       </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V104" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (5.561); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -7156,6 +7356,16 @@
       <c r="T109" s="2">
         <v>45819</v>
       </c>
+      <c r="U109" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V109" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (2.627); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -7271,6 +7481,16 @@
       <c r="T111" s="2">
         <v>45821</v>
       </c>
+      <c r="U111" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V111" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (3.842); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -7690,6 +7910,16 @@
       <c r="T118" s="2">
         <v>45821</v>
       </c>
+      <c r="U118" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V118" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (4.696); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -8114,6 +8344,16 @@
       <c r="T125" s="2">
         <v>45821</v>
       </c>
+      <c r="U125" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V125" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (5.85); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -8692,6 +8932,16 @@
       <c r="T135" s="2">
         <v>45845</v>
       </c>
+      <c r="U135" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V135" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.017); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -9944,6 +10194,16 @@
       <c r="T155" s="2">
         <v>45845</v>
       </c>
+      <c r="U155" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V155" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (9.705); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -10463,6 +10723,16 @@
       <c r="T163" s="2">
         <v>45835</v>
       </c>
+      <c r="U163" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V163" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.317); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -10523,6 +10793,16 @@
       <c r="T164" s="2">
         <v>45835</v>
       </c>
+      <c r="U164" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V164" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (1.219); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -10583,6 +10863,16 @@
       <c r="T165" s="2">
         <v>45833</v>
       </c>
+      <c r="U165" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V165" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-12.128); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -10643,6 +10933,16 @@
       <c r="T166" s="2">
         <v>45845</v>
       </c>
+      <c r="U166" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V166" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-2.484); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -10812,6 +11112,16 @@
       <c r="T169" s="2">
         <v>45860</v>
       </c>
+      <c r="U169" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V169" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (7.382); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -11226,6 +11536,16 @@
       <c r="T176" s="2">
         <v>45860</v>
       </c>
+      <c r="U176" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V176" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (6.489); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -11685,6 +12005,16 @@
       <c r="T184" s="2">
         <v>45845</v>
       </c>
+      <c r="U184" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V184" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.9); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -13436,6 +13766,16 @@
       <c r="T212" s="2">
         <v>45869</v>
       </c>
+      <c r="U212" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V212" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.009); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -13496,6 +13836,16 @@
       <c r="T213" s="2">
         <v>45867</v>
       </c>
+      <c r="U213" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V213" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.813); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -13613,6 +13963,16 @@
       <c r="T215" s="2">
         <v>45860</v>
       </c>
+      <c r="U215" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V215" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (2.644); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -13673,6 +14033,16 @@
       <c r="T216" s="2">
         <v>45863</v>
       </c>
+      <c r="U216" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V216" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (3.034); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -13733,6 +14103,16 @@
       <c r="T217" s="2">
         <v>45875</v>
       </c>
+      <c r="U217" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V217" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (5.066); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -13905,6 +14285,16 @@
       <c r="T220" s="2">
         <v>45863</v>
       </c>
+      <c r="U220" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V220" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (4.716); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -13965,6 +14355,16 @@
       <c r="T221" s="2">
         <v>45860</v>
       </c>
+      <c r="U221" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V221" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (4.776); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -14369,6 +14769,16 @@
       <c r="T228" s="2">
         <v>45863</v>
       </c>
+      <c r="U228" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V228" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (5.195); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -14553,6 +14963,16 @@
       <c r="T231" s="2">
         <v>45866</v>
       </c>
+      <c r="U231" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V231" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (7.883); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -14858,6 +15278,16 @@
       <c r="T236" s="2">
         <v>45860</v>
       </c>
+      <c r="U236" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V236" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (5.068); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -16010,6 +16440,16 @@
       <c r="T254" s="2">
         <v>45875</v>
       </c>
+      <c r="U254" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V254" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.193); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -16070,6 +16510,16 @@
       <c r="T255" s="2">
         <v>45875</v>
       </c>
+      <c r="U255" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V255" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.552); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -16187,6 +16637,16 @@
       <c r="T257" s="2">
         <v>45881</v>
       </c>
+      <c r="U257" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V257" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (2.204); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -16247,6 +16707,16 @@
       <c r="T258" s="2">
         <v>45880</v>
       </c>
+      <c r="U258" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V258" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (2.534); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -16364,6 +16834,16 @@
       <c r="T260" s="2">
         <v>45883</v>
       </c>
+      <c r="U260" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V260" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-8.883); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -16479,6 +16959,16 @@
       <c r="T262" s="2">
         <v>45880</v>
       </c>
+      <c r="U262" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V262" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-3.565); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -16594,6 +17084,16 @@
       <c r="T264" s="2">
         <v>45881</v>
       </c>
+      <c r="U264" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V264" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (6.875); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -17003,6 +17503,16 @@
       <c r="T271" s="2">
         <v>45880</v>
       </c>
+      <c r="U271" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V271" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (4.597); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -17247,6 +17757,16 @@
       <c r="T275" s="2">
         <v>45880</v>
       </c>
+      <c r="U275" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V275" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-1.929); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -17871,6 +18391,16 @@
       <c r="T285" s="2">
         <v>45880</v>
       </c>
+      <c r="U285" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V285" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-3.654); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -18265,6 +18795,16 @@
       <c r="T291" s="2">
         <v>45880</v>
       </c>
+      <c r="U291" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V291" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-2.373); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -18584,6 +19124,16 @@
       <c r="T296" s="2">
         <v>45895</v>
       </c>
+      <c r="U296" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V296" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-1.037); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -18754,6 +19304,16 @@
       <c r="T299" s="2">
         <v>45897</v>
       </c>
+      <c r="U299" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V299" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (6.932); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -18983,6 +19543,16 @@
       <c r="T303" s="2">
         <v>45895</v>
       </c>
+      <c r="U303" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V303" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-1.172); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -19412,6 +19982,16 @@
       <c r="T310" s="2">
         <v>45895</v>
       </c>
+      <c r="U310" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V310" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.244); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -19841,6 +20421,16 @@
       <c r="T317" s="2">
         <v>45895</v>
       </c>
+      <c r="U317" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V317" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.48); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -20365,6 +20955,16 @@
       <c r="T325" s="2">
         <v>45895</v>
       </c>
+      <c r="U325" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V325" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-1.509); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -20879,6 +21479,16 @@
       <c r="T333" s="2">
         <v>45910</v>
       </c>
+      <c r="U333" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V333" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.047); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -20939,6 +21549,16 @@
       <c r="T334" s="2">
         <v>45895</v>
       </c>
+      <c r="U334" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V334" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (2.406); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -21116,6 +21736,16 @@
       <c r="T337" s="2">
         <v>45896</v>
       </c>
+      <c r="U337" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V337" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-32.857); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -21176,6 +21806,16 @@
       <c r="T338" s="2">
         <v>45897</v>
       </c>
+      <c r="U338" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V338" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (4.537); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -21363,6 +22003,16 @@
       <c r="T341" s="2">
         <v>45917</v>
       </c>
+      <c r="U341" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V341" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-11.577); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -21493,6 +22143,16 @@
       <c r="T343" s="2">
         <v>45930</v>
       </c>
+      <c r="U343" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V343" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-22.585); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -21620,6 +22280,16 @@
       <c r="T345" s="2">
         <v>45916</v>
       </c>
+      <c r="U345" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V345" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (3.796); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -21747,6 +22417,16 @@
       <c r="T347" s="2">
         <v>45930</v>
       </c>
+      <c r="U347" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V347" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-21.388); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -22296,6 +22976,16 @@
       <c r="T356" s="2">
         <v>45930</v>
       </c>
+      <c r="U356" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V356" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-22.136); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -22780,6 +23470,16 @@
       <c r="T364" s="2">
         <v>45915</v>
       </c>
+      <c r="U364" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V364" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (5.637); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -23024,6 +23724,16 @@
       <c r="T368" s="2">
         <v>45915</v>
       </c>
+      <c r="U368" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V368" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (3.204); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -23508,6 +24218,16 @@
       <c r="T376" s="2">
         <v>45915</v>
       </c>
+      <c r="U376" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V376" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (2.958); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -23987,6 +24707,16 @@
       <c r="T384" s="2">
         <v>45918</v>
       </c>
+      <c r="U384" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V384" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.606); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -24164,6 +24894,16 @@
       <c r="T387" s="2">
         <v>45919</v>
       </c>
+      <c r="U387" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V387" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (3.137); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -24224,6 +24964,16 @@
       <c r="T388" s="2">
         <v>45936</v>
       </c>
+      <c r="U388" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V388" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-33.03); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -24284,6 +25034,16 @@
       <c r="T389" s="2">
         <v>45927</v>
       </c>
+      <c r="U389" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V389" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (4.242); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -24461,6 +25221,16 @@
       <c r="T392" s="2">
         <v>45919</v>
       </c>
+      <c r="U392" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V392" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (4.816); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -24985,6 +25755,16 @@
       <c r="T401" s="2">
         <v>45919</v>
       </c>
+      <c r="U401" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V401" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (6.82); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
@@ -25349,6 +26129,16 @@
       <c r="T407" s="2">
         <v>45919</v>
       </c>
+      <c r="U407" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V407" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (2.106); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
@@ -25658,6 +26448,16 @@
       <c r="T412" s="2">
         <v>45919</v>
       </c>
+      <c r="U412" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V412" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (1.095); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
@@ -26439,6 +27239,16 @@
       <c r="T424" s="2">
         <v>45919</v>
       </c>
+      <c r="U424" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V424" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (4.148); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
@@ -26566,6 +27376,16 @@
       <c r="T426" s="2">
         <v>45930</v>
       </c>
+      <c r="U426" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V426" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.109); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
@@ -26866,6 +27686,16 @@
       <c r="T431" s="2">
         <v>45936</v>
       </c>
+      <c r="U431" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V431" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-27.681); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
@@ -26986,6 +27816,16 @@
       <c r="T433" s="2">
         <v>45930</v>
       </c>
+      <c r="U433" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V433" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-1.443); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
@@ -27831,6 +28671,16 @@
       <c r="T447" s="2">
         <v>45930</v>
       </c>
+      <c r="U447" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V447" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (1.847); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="448">
       <c r="A448" t="inlineStr">
@@ -28271,6 +29121,16 @@
       <c r="T454" s="2">
         <v>45930</v>
       </c>
+      <c r="U454" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V454" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (0.296); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
@@ -28741,6 +29601,16 @@
       <c r="T461" s="2">
         <v>45930</v>
       </c>
+      <c r="U461" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V461" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.714); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
@@ -29201,6 +30071,16 @@
       <c r="T468" s="2">
         <v>45946</v>
       </c>
+      <c r="U468" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V468" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.683); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
@@ -29916,6 +30796,16 @@
       <c r="T480" s="2">
         <v>45946</v>
       </c>
+      <c r="U480" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V480" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (8.081); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
@@ -31396,6 +32286,16 @@
       <c r="T503" s="2">
         <v>45951</v>
       </c>
+      <c r="U503" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V503" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.054); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="504">
       <c r="A504" t="inlineStr">
@@ -31456,6 +32356,16 @@
       <c r="T504" s="2">
         <v>45951</v>
       </c>
+      <c r="U504" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V504" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-0.65); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="505">
       <c r="A505" t="inlineStr">
@@ -31576,6 +32486,16 @@
       <c r="T506" s="2">
         <v>45980</v>
       </c>
+      <c r="U506" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V506" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-21.802); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="507">
       <c r="A507" t="inlineStr">
@@ -31811,6 +32731,16 @@
       <c r="T510" s="2">
         <v>45968</v>
       </c>
+      <c r="U510" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V510" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (1.135); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
@@ -31871,6 +32801,16 @@
       <c r="T511" s="2">
         <v>45972</v>
       </c>
+      <c r="U511" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V511" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-1.824); replaced with &lt;lod</t>
+        </is>
+      </c>
     </row>
     <row r="512">
       <c r="A512" t="inlineStr">
@@ -31990,6 +32930,16 @@
       </c>
       <c r="T513" s="2">
         <v>45980</v>
+      </c>
+      <c r="U513" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="V513" t="inlineStr">
+        <is>
+          <t>Result &lt; LOD (-22.365); replaced with &lt;lod</t>
+        </is>
       </c>
     </row>
     <row r="514">

</xml_diff>